<commit_message>
Se implementó backpropagation con inercia. Se hicieron pruebas con un conjunto de entrenamiento de 50000 imagenes, 30 epochs, minibatches de tamaño 10, eta=7.5 (el valor que dio mejor resultado para la red basica) y valores de mu: 0.4,0.5,0.6,0.7,0.8 y 0.9. El valor que dio mejores resultados fue mu=0.9, llegando a un 93.40% de aciertos en el conjunto de validacion (10000 imagenes) y un 92.93% de aciertos en el conjunto de prueba (10000 imagenes), valor que fue menor al obtenido con la red basica. Por otro lado, se observo que el aprendizaje con este algoritmo y mu=0.9 fue mas rapido que el de la red basica.
</commit_message>
<xml_diff>
--- a/Observaciones.xlsx
+++ b/Observaciones.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jorge\Documents\DataScience\RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C33372-0B14-4B26-AB28-EF3BF12A7AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC97228-4849-47F6-A069-FFFA8D172ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD371440-6D23-4AFF-826B-EDAE8CF93875}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{AD371440-6D23-4AFF-826B-EDAE8CF93875}"/>
   </bookViews>
   <sheets>
     <sheet name="Red básica" sheetId="1" r:id="rId1"/>
+    <sheet name="Red con inercia" sheetId="2" r:id="rId2"/>
+    <sheet name="Red con Cross entropy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>Epochs</t>
   </si>
@@ -77,6 +79,27 @@
   </si>
   <si>
     <t>Precisión en datos de validación del 92.94%.</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 92.95%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 73.06%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 92.68%</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 83.41%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 92.91%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 93.40%.</t>
   </si>
 </sst>
 </file>
@@ -138,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,7 +185,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4746188-008C-445C-8751-A884F7D283D6}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,18 +677,222 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8276372-4984-42E1-A8A8-5C8992CD95B8}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="86.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B5" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B7" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259820BF-CF16-48EB-A301-36087F0B1400}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se implementó cross entropy. Se hicieron pruebas con un conjunto de entrenamiento de 50000 imagenes, 30 epochs, minibatches de tamaño 10, valores de eta: 15.0, 7.5, 4.0, 2.0, 1.0 y 0.5, y valores de mu: 1.0, 0.8 y 0.9. La combinacion de valores que dio mejores resultados fue eta=0.5 y mu=0.9, llegando a un 93.83% de aciertos en el conjunto de validacion (10000 imagenes) y un 93.79% de aciertos en el conjunto de prueba (10000 imagenes), valor que fue mayor a los obtenidos con la red basica (93.4% de aciertos en conjunto de prueba) y la red con back propagation con inercia (92.93% de aciertos en conjunto de prueba). Una observacion interesante es que varias combinaciones de valores de eta y mu dieron valores de porcentaje de aciertos muy cercanos al obtenido con la mejor combinacion.
</commit_message>
<xml_diff>
--- a/Observaciones.xlsx
+++ b/Observaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jorge\Documents\DataScience\RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC97228-4849-47F6-A069-FFFA8D172ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B031BAC8-BC90-416B-BDAF-5D7D03A9BD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{AD371440-6D23-4AFF-826B-EDAE8CF93875}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{AD371440-6D23-4AFF-826B-EDAE8CF93875}"/>
   </bookViews>
   <sheets>
     <sheet name="Red básica" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t>Epochs</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Precisión en datos de validación del 94.29%, indica que el paso de aprendizaje es adecuado.</t>
   </si>
   <si>
-    <t>Precisión en datos de validación del 10.09%, se encontró mucho sobreajuste.</t>
-  </si>
-  <si>
     <t>Precisión en datos de validación del 93.61%.</t>
   </si>
   <si>
@@ -100,6 +97,48 @@
   </si>
   <si>
     <t>Precisión en datos de validación del 93.40%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 48.45%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 59.85%</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 89.36%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 92.89%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 91.86%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 94.19%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 88.93%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 94.18%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 93.83%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 94.15%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 94.10%.</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 93.58%.</t>
+  </si>
+  <si>
+    <t>Porcentaje de aciertos en conjunto de prueba</t>
+  </si>
+  <si>
+    <t>Precisión en datos de validación del 10.09%.</t>
   </si>
 </sst>
 </file>
@@ -129,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +187,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -161,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,6 +229,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4746188-008C-445C-8751-A884F7D283D6}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +616,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -651,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -674,7 +731,7 @@
         <v>0.5</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -688,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8276372-4984-42E1-A8A8-5C8992CD95B8}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -747,7 +804,7 @@
         <v>0.4</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -773,7 +830,7 @@
         <v>0.5</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,7 +856,7 @@
         <v>0.6</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -825,7 +882,7 @@
         <v>0.7</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -851,7 +908,7 @@
         <v>0.8</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -877,7 +934,7 @@
         <v>0.9</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -887,12 +944,394 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259820BF-CF16-48EB-A301-36087F0B1400}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="A10:I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" customWidth="1"/>
+    <col min="9" max="9" width="42" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
+        <v>15</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <v>4</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B5" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6">
+        <v>2</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.93820000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B7" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B9" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4">
+        <v>10</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.93759999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.93789999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>30</v>
+      </c>
+      <c r="E11" s="4">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0.93669999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B13" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4">
+        <v>10</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>